<commit_message>
börjat med datahanterin, i luv u
</commit_message>
<xml_diff>
--- a/checkPoints_graduation/coursesM.xlsx
+++ b/checkPoints_graduation/coursesM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filipbirkfeldt/git/easyplan/checkPoints_graduation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B973FABF-09A2-2F43-BEF0-65DD790DD687}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9CE631-4F21-2140-BF11-DBAE7AF118AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{88FF2B37-B084-954A-BA13-F008CFE814E1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32020" windowHeight="21100" xr2:uid="{88FF2B37-B084-954A-BA13-F008CFE814E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="142">
-  <si>
-    <t>Kurs­kod</t>
-  </si>
   <si>
     <t>Poäng</t>
   </si>
@@ -762,6 +759,9 @@
       </rPr>
       <t>T</t>
     </r>
+  </si>
+  <si>
+    <t>Kurskod</t>
   </si>
 </sst>
 </file>
@@ -1187,13 +1187,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA98A3B-A755-4B47-9CD8-6AB1CD7C4B17}">
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="6" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="61.83203125" bestFit="1" customWidth="1"/>
@@ -1202,58 +1200,58 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -1262,17 +1260,17 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="5">
@@ -1284,13 +1282,13 @@
     </row>
     <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -1299,19 +1297,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1323,34 +1321,34 @@
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4">
         <v>7.5</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="5">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="5">
@@ -1362,32 +1360,32 @@
     </row>
     <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4">
-        <v>4</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="5">
@@ -1399,32 +1397,32 @@
     </row>
     <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B6" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5">
-        <v>4</v>
-      </c>
-      <c r="E6" s="4">
-        <v>4</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="5">
@@ -1436,13 +1434,13 @@
     </row>
     <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4">
         <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5">
         <v>4</v>
@@ -1451,17 +1449,17 @@
         <v>3</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="5">
@@ -1473,32 +1471,32 @@
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4">
-        <v>4</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="5">
@@ -1510,13 +1508,13 @@
     </row>
     <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="5">
         <v>4</v>
@@ -1525,17 +1523,17 @@
         <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="5">
@@ -1547,32 +1545,32 @@
     </row>
     <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B10" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5">
-        <v>4</v>
-      </c>
-      <c r="E10" s="4">
-        <v>3</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="5">
@@ -1584,13 +1582,13 @@
     </row>
     <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5">
         <v>4</v>
@@ -1599,17 +1597,17 @@
         <v>3</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="5">
@@ -1621,34 +1619,34 @@
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="5">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="5">
-        <v>4</v>
-      </c>
-      <c r="E12" s="4">
-        <v>3</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="I12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="5">
@@ -1660,32 +1658,32 @@
     </row>
     <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4</v>
+      </c>
+      <c r="E13" s="4">
+        <v>4</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B13" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="5">
-        <v>4</v>
-      </c>
-      <c r="E13" s="4">
-        <v>4</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="5">
@@ -1697,32 +1695,32 @@
     </row>
     <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="B14" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="5">
-        <v>4</v>
-      </c>
-      <c r="E14" s="4">
-        <v>4</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="5">
@@ -1734,32 +1732,32 @@
     </row>
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="5">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B15" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="5">
-        <v>4</v>
-      </c>
-      <c r="E15" s="4">
-        <v>3</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="5">
@@ -1771,34 +1769,34 @@
     </row>
     <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4</v>
+      </c>
+      <c r="E16" s="4">
+        <v>4</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="5">
-        <v>4</v>
-      </c>
-      <c r="E16" s="4">
-        <v>4</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="I16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="5">
@@ -1810,32 +1808,32 @@
     </row>
     <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="B17" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4</v>
-      </c>
-      <c r="E17" s="4">
-        <v>4</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="5">
@@ -1847,34 +1845,34 @@
     </row>
     <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="5">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4">
+        <v>4</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="5">
-        <v>4</v>
-      </c>
-      <c r="E18" s="4">
-        <v>4</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="I18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="5">
@@ -1886,32 +1884,32 @@
     </row>
     <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="5">
+        <v>4</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B19" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="5">
-        <v>4</v>
-      </c>
-      <c r="E19" s="4">
-        <v>3</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="5">
@@ -1923,32 +1921,32 @@
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="5">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B20" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="5">
-        <v>4</v>
-      </c>
-      <c r="E20" s="4">
-        <v>3</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="5">
@@ -1960,32 +1958,32 @@
     </row>
     <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="5">
+        <v>4</v>
+      </c>
+      <c r="E21" s="4">
+        <v>4</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B21" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="5">
-        <v>4</v>
-      </c>
-      <c r="E21" s="4">
-        <v>4</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="5">
@@ -1999,32 +1997,32 @@
     </row>
     <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="5">
+        <v>4</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="B22" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="5">
-        <v>4</v>
-      </c>
-      <c r="E22" s="4">
-        <v>3</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="5">
@@ -2038,32 +2036,32 @@
     </row>
     <row r="23" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4</v>
+      </c>
+      <c r="E23" s="4">
+        <v>3</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="B23" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="5">
-        <v>4</v>
-      </c>
-      <c r="E23" s="4">
-        <v>3</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="5">
@@ -2077,32 +2075,32 @@
     </row>
     <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B24" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="5">
-        <v>4</v>
-      </c>
-      <c r="E24" s="4">
-        <v>3</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="5">
@@ -2116,32 +2114,32 @@
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4</v>
+      </c>
+      <c r="E25" s="4">
+        <v>4</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B25" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="5">
-        <v>4</v>
-      </c>
-      <c r="E25" s="4">
-        <v>4</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="5">
@@ -2155,32 +2153,32 @@
     </row>
     <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B26" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="5">
-        <v>4</v>
-      </c>
-      <c r="E26" s="4">
-        <v>4</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -2192,32 +2190,32 @@
     </row>
     <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B27" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="5">
-        <v>4</v>
-      </c>
-      <c r="E27" s="4">
-        <v>3</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -2229,32 +2227,32 @@
     </row>
     <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5">
+        <v>4</v>
+      </c>
+      <c r="E28" s="4">
+        <v>4</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B28" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="5">
-        <v>4</v>
-      </c>
-      <c r="E28" s="4">
-        <v>4</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -2266,34 +2264,34 @@
     </row>
     <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="5">
+        <v>4</v>
+      </c>
+      <c r="E29" s="4">
+        <v>4</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="5">
-        <v>4</v>
-      </c>
-      <c r="E29" s="4">
-        <v>4</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="I29" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -2305,32 +2303,32 @@
     </row>
     <row r="30" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="5">
+        <v>4</v>
+      </c>
+      <c r="E30" s="4">
+        <v>4</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="B30" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="5">
-        <v>4</v>
-      </c>
-      <c r="E30" s="4">
-        <v>4</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -2342,13 +2340,13 @@
     </row>
     <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="4">
         <v>15</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="5">
         <v>4</v>
@@ -2357,17 +2355,17 @@
         <v>3</v>
       </c>
       <c r="F31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H31" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -2379,13 +2377,13 @@
     </row>
     <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="4">
         <v>7.5</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="5">
         <v>4</v>
@@ -2394,17 +2392,17 @@
         <v>2</v>
       </c>
       <c r="F32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H32" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -2416,13 +2414,13 @@
     </row>
     <row r="33" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="4">
         <v>7</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" s="5">
         <v>4</v>
@@ -2431,17 +2429,17 @@
         <v>2</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -2453,13 +2451,13 @@
     </row>
     <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" s="4">
         <v>6</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" s="5">
         <v>4</v>
@@ -2468,17 +2466,17 @@
         <v>4</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -2490,34 +2488,34 @@
     </row>
     <row r="35" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4</v>
+      </c>
+      <c r="E35" s="4">
+        <v>3</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="5">
-        <v>4</v>
-      </c>
-      <c r="E35" s="4">
-        <v>3</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="I35" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -2529,32 +2527,32 @@
     </row>
     <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="5">
+        <v>4</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B36" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="5">
-        <v>4</v>
-      </c>
-      <c r="E36" s="4">
-        <v>4</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -2566,32 +2564,32 @@
     </row>
     <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="5">
+        <v>4</v>
+      </c>
+      <c r="E37" s="4">
+        <v>4</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="B37" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="5">
-        <v>4</v>
-      </c>
-      <c r="E37" s="4">
-        <v>4</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -2603,32 +2601,32 @@
     </row>
     <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="5">
+        <v>4</v>
+      </c>
+      <c r="E38" s="4">
+        <v>3</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B38" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="5">
-        <v>4</v>
-      </c>
-      <c r="E38" s="4">
-        <v>3</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -2640,13 +2638,13 @@
     </row>
     <row r="39" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="4">
         <v>15</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D39" s="5">
         <v>4</v>
@@ -2655,17 +2653,17 @@
         <v>3</v>
       </c>
       <c r="F39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H39" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
@@ -2677,34 +2675,34 @@
     </row>
     <row r="40" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="5">
+        <v>4</v>
+      </c>
+      <c r="E40" s="4">
+        <v>3</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="5">
-        <v>4</v>
-      </c>
-      <c r="E40" s="4">
-        <v>3</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="I40" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
@@ -2716,13 +2714,13 @@
     </row>
     <row r="41" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="4">
         <v>7</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" s="5">
         <v>4</v>
@@ -2731,17 +2729,17 @@
         <v>2</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G41" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
@@ -2753,32 +2751,32 @@
     </row>
     <row r="42" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="5">
+        <v>4</v>
+      </c>
+      <c r="E42" s="4">
+        <v>3</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="B42" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="5">
-        <v>4</v>
-      </c>
-      <c r="E42" s="4">
-        <v>3</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
@@ -2790,32 +2788,32 @@
     </row>
     <row r="43" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="5">
+        <v>4</v>
+      </c>
+      <c r="E43" s="4">
+        <v>4</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="B43" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="5">
-        <v>4</v>
-      </c>
-      <c r="E43" s="4">
-        <v>4</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
@@ -2827,34 +2825,34 @@
     </row>
     <row r="44" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="5">
+        <v>4</v>
+      </c>
+      <c r="E44" s="4">
+        <v>3</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="5">
-        <v>4</v>
-      </c>
-      <c r="E44" s="4">
-        <v>3</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="I44" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
@@ -2866,34 +2864,34 @@
     </row>
     <row r="45" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="5">
+        <v>4</v>
+      </c>
+      <c r="E45" s="4">
+        <v>3</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="5">
-        <v>4</v>
-      </c>
-      <c r="E45" s="4">
-        <v>3</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="I45" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
@@ -2905,32 +2903,32 @@
     </row>
     <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="5">
+        <v>4</v>
+      </c>
+      <c r="E46" s="4">
+        <v>4</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B46" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="5">
-        <v>4</v>
-      </c>
-      <c r="E46" s="4">
-        <v>4</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
@@ -2942,32 +2940,32 @@
     </row>
     <row r="47" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="5">
+        <v>4</v>
+      </c>
+      <c r="E47" s="4">
+        <v>4</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H47" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="B47" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" s="5">
-        <v>4</v>
-      </c>
-      <c r="E47" s="4">
-        <v>4</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
@@ -2979,32 +2977,32 @@
     </row>
     <row r="48" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="5">
+        <v>4</v>
+      </c>
+      <c r="E48" s="4">
+        <v>3</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H48" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B48" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="5">
-        <v>4</v>
-      </c>
-      <c r="E48" s="4">
-        <v>3</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
@@ -3016,32 +3014,32 @@
     </row>
     <row r="49" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="5">
+        <v>4</v>
+      </c>
+      <c r="E49" s="4">
+        <v>3</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B49" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="5">
-        <v>4</v>
-      </c>
-      <c r="E49" s="4">
-        <v>3</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
@@ -3053,32 +3051,32 @@
     </row>
     <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="5">
+        <v>4</v>
+      </c>
+      <c r="E50" s="4">
+        <v>4</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="B50" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50" s="5">
-        <v>4</v>
-      </c>
-      <c r="E50" s="4">
-        <v>4</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -3090,32 +3088,32 @@
     </row>
     <row r="51" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="5">
+        <v>4</v>
+      </c>
+      <c r="E51" s="4">
+        <v>4</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H51" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="B51" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D51" s="5">
-        <v>4</v>
-      </c>
-      <c r="E51" s="4">
-        <v>4</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -3127,32 +3125,32 @@
     </row>
     <row r="52" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="5">
+        <v>4</v>
+      </c>
+      <c r="E52" s="4">
+        <v>4</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B52" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="5">
-        <v>4</v>
-      </c>
-      <c r="E52" s="4">
-        <v>4</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -3164,13 +3162,13 @@
     </row>
     <row r="53" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="4">
         <v>5</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D53" s="5">
         <v>4</v>
@@ -3179,17 +3177,17 @@
         <v>3</v>
       </c>
       <c r="F53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G53" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H53" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -3201,32 +3199,32 @@
     </row>
     <row r="54" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="5">
+        <v>4</v>
+      </c>
+      <c r="E54" s="4">
+        <v>4</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H54" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B54" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D54" s="5">
-        <v>4</v>
-      </c>
-      <c r="E54" s="4">
-        <v>4</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -3240,32 +3238,32 @@
     </row>
     <row r="55" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="5">
+        <v>4</v>
+      </c>
+      <c r="E55" s="4">
+        <v>4</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B55" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D55" s="5">
-        <v>4</v>
-      </c>
-      <c r="E55" s="4">
-        <v>4</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="I55" s="4"/>
       <c r="J55" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -3279,32 +3277,32 @@
     </row>
     <row r="56" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="5">
+        <v>4</v>
+      </c>
+      <c r="E56" s="4">
+        <v>4</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="B56" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" s="5">
-        <v>4</v>
-      </c>
-      <c r="E56" s="4">
-        <v>4</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="I56" s="4"/>
       <c r="J56" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -3318,32 +3316,32 @@
     </row>
     <row r="57" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="5">
+        <v>4</v>
+      </c>
+      <c r="E57" s="4">
+        <v>3</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="B57" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D57" s="5">
-        <v>4</v>
-      </c>
-      <c r="E57" s="4">
-        <v>3</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
@@ -3357,32 +3355,32 @@
     </row>
     <row r="58" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="5">
+        <v>4</v>
+      </c>
+      <c r="E58" s="4">
+        <v>3</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="B58" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D58" s="5">
-        <v>4</v>
-      </c>
-      <c r="E58" s="4">
-        <v>3</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
@@ -3396,32 +3394,32 @@
     </row>
     <row r="59" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="5">
+        <v>4</v>
+      </c>
+      <c r="E59" s="4">
+        <v>3</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H59" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="B59" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="5">
-        <v>4</v>
-      </c>
-      <c r="E59" s="4">
-        <v>3</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
@@ -3435,32 +3433,32 @@
     </row>
     <row r="60" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="5">
+        <v>4</v>
+      </c>
+      <c r="E60" s="4">
+        <v>3</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B60" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D60" s="5">
-        <v>4</v>
-      </c>
-      <c r="E60" s="4">
-        <v>3</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="I60" s="4"/>
       <c r="J60" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
@@ -3474,32 +3472,32 @@
     </row>
     <row r="61" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="5">
+        <v>4</v>
+      </c>
+      <c r="E61" s="4">
+        <v>4</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H61" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B61" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D61" s="5">
-        <v>4</v>
-      </c>
-      <c r="E61" s="4">
-        <v>4</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -3513,32 +3511,32 @@
     </row>
     <row r="62" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" s="5">
+        <v>4</v>
+      </c>
+      <c r="E62" s="4">
+        <v>3</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B62" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D62" s="5">
-        <v>4</v>
-      </c>
-      <c r="E62" s="4">
-        <v>3</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
@@ -3550,13 +3548,13 @@
     </row>
     <row r="63" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B63" s="4">
         <v>15</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D63" s="5">
         <v>4</v>
@@ -3565,17 +3563,17 @@
         <v>3</v>
       </c>
       <c r="F63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G63" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H63" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I63" s="4"/>
       <c r="J63" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
@@ -3587,13 +3585,13 @@
     </row>
     <row r="64" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64" s="4">
         <v>7</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D64" s="5">
         <v>4</v>
@@ -3602,17 +3600,17 @@
         <v>2</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I64" s="4"/>
       <c r="J64" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
@@ -3624,13 +3622,13 @@
     </row>
     <row r="65" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="4">
         <v>6</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D65" s="5">
         <v>4</v>
@@ -3639,17 +3637,17 @@
         <v>4</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
@@ -3661,32 +3659,32 @@
     </row>
     <row r="66" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="5">
+        <v>4</v>
+      </c>
+      <c r="E66" s="4">
+        <v>4</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H66" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="B66" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D66" s="5">
-        <v>4</v>
-      </c>
-      <c r="E66" s="4">
-        <v>4</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H66" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
@@ -3698,34 +3696,34 @@
     </row>
     <row r="67" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="5">
+        <v>4</v>
+      </c>
+      <c r="E67" s="4">
+        <v>3</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H67" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B67" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D67" s="5">
-        <v>4</v>
-      </c>
-      <c r="E67" s="4">
-        <v>3</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="I67" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
@@ -3737,32 +3735,32 @@
     </row>
     <row r="68" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D68" s="5">
+        <v>4</v>
+      </c>
+      <c r="E68" s="4">
+        <v>4</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B68" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="5">
-        <v>4</v>
-      </c>
-      <c r="E68" s="4">
-        <v>4</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="I68" s="4"/>
       <c r="J68" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
@@ -3774,32 +3772,32 @@
     </row>
     <row r="69" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B69" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="5">
+        <v>4</v>
+      </c>
+      <c r="E69" s="4">
+        <v>4</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H69" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="B69" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D69" s="5">
-        <v>4</v>
-      </c>
-      <c r="E69" s="4">
-        <v>4</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H69" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="I69" s="4"/>
       <c r="J69" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
@@ -3811,32 +3809,32 @@
     </row>
     <row r="70" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B70" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="5">
+        <v>4</v>
+      </c>
+      <c r="E70" s="4">
+        <v>3</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B70" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D70" s="5">
-        <v>4</v>
-      </c>
-      <c r="E70" s="4">
-        <v>3</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="I70" s="4"/>
       <c r="J70" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
@@ -3848,13 +3846,13 @@
     </row>
     <row r="71" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B71" s="4">
         <v>2</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D71" s="5">
         <v>4</v>
@@ -3863,17 +3861,17 @@
         <v>3</v>
       </c>
       <c r="F71" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G71" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H71" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
@@ -3885,32 +3883,32 @@
     </row>
     <row r="72" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B72" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="5">
+        <v>4</v>
+      </c>
+      <c r="E72" s="4">
+        <v>4</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H72" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="B72" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D72" s="5">
-        <v>4</v>
-      </c>
-      <c r="E72" s="4">
-        <v>4</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="I72" s="4"/>
       <c r="J72" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
@@ -3922,34 +3920,34 @@
     </row>
     <row r="73" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="5">
+        <v>4</v>
+      </c>
+      <c r="E73" s="4">
+        <v>4</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H73" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B73" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D73" s="5">
-        <v>4</v>
-      </c>
-      <c r="E73" s="4">
-        <v>4</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="I73" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
@@ -3961,32 +3959,32 @@
     </row>
     <row r="74" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="5">
+        <v>4</v>
+      </c>
+      <c r="E74" s="4">
+        <v>4</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H74" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="B74" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D74" s="5">
-        <v>4</v>
-      </c>
-      <c r="E74" s="4">
-        <v>4</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="I74" s="4"/>
       <c r="J74" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
@@ -3998,32 +3996,32 @@
     </row>
     <row r="75" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B75" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="5">
+        <v>4</v>
+      </c>
+      <c r="E75" s="4">
+        <v>3</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H75" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="B75" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D75" s="5">
-        <v>4</v>
-      </c>
-      <c r="E75" s="4">
-        <v>3</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
@@ -4035,13 +4033,13 @@
     </row>
     <row r="76" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B76" s="4">
         <v>7.5</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D76" s="5">
         <v>5</v>
@@ -4050,19 +4048,19 @@
         <v>4</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K76" s="4"/>
       <c r="L76" s="5">
@@ -4074,13 +4072,13 @@
     </row>
     <row r="77" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B77" s="4">
         <v>7.5</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D77" s="5">
         <v>5</v>
@@ -4089,17 +4087,17 @@
         <v>5</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I77" s="4"/>
       <c r="J77" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K77" s="4"/>
       <c r="L77" s="5">
@@ -4113,13 +4111,13 @@
     </row>
     <row r="78" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B78" s="4">
         <v>7.5</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D78" s="5">
         <v>5</v>
@@ -4128,17 +4126,17 @@
         <v>4</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I78" s="4"/>
       <c r="J78" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
@@ -4150,13 +4148,13 @@
     </row>
     <row r="79" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B79" s="4">
         <v>7.5</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D79" s="5">
         <v>5</v>
@@ -4165,19 +4163,19 @@
         <v>4</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
@@ -4189,11 +4187,11 @@
     </row>
     <row r="80" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -4206,11 +4204,11 @@
     </row>
     <row r="81" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -4223,34 +4221,34 @@
     </row>
     <row r="82" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B82" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82" s="8">
+        <v>4</v>
+      </c>
+      <c r="E82" s="7">
+        <v>3</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H82" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B82" s="7">
-        <v>7.5</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D82" s="8">
-        <v>4</v>
-      </c>
-      <c r="E82" s="7">
-        <v>3</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H82" s="7" t="s">
+      <c r="I82" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J82" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="I82" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J82" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="K82" s="7"/>
     </row>

</xml_diff>